<commit_message>
Munger re-design - BOM - wip
</commit_message>
<xml_diff>
--- a/modules/Wavefolder/Wavefolder-BOM.xlsx
+++ b/modules/Wavefolder/Wavefolder-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Wavefolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D237BE99-6D0B-452A-BC9C-EE14150F13DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A964A-1B69-4E96-8436-50181BCBC4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9870" yWindow="2280" windowWidth="18540" windowHeight="12495"/>
+    <workbookView xWindow="5940" yWindow="1260" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wavefolder-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="199">
   <si>
     <t>Ref</t>
   </si>
@@ -163,12 +176,6 @@
     <t>C101 C102</t>
   </si>
   <si>
-    <t>CP_10U</t>
-  </si>
-  <si>
-    <t>35 VDC</t>
-  </si>
-  <si>
     <t>12 V decoupling</t>
   </si>
   <si>
@@ -364,31 +371,43 @@
     <t>499K</t>
   </si>
   <si>
+    <t>1%, 1/4 W</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/447/YAGEO_MFR_datasheet_2023v3-3324391.pdf</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>MFR-25FTE52-499K</t>
+  </si>
+  <si>
+    <t>603-MFR-25FTE52-499K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FTE52-499K?qs=oAGoVhmvjhyZIgXtFNjfqg%3D%3D</t>
+  </si>
+  <si>
+    <t>R2 R15 R17 R30</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
     <t>1%, 1/6 W</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/datasheet/2/447/YAGEO_MFR_datasheet_2023v3-3324391.pdf</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
-    <t>MFR-12*</t>
-  </si>
-  <si>
-    <t>603-MFR-12*</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/c/?m=YAGEO&amp;power+rating=166+mW+(1%2f6+W)&amp;tolerance=1+%25&amp;instock=y</t>
-  </si>
-  <si>
-    <t>R2 R15 R17 R30</t>
-  </si>
-  <si>
-    <t>100K</t>
+    <t>MFR-12FTF52-100K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-100K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-100K?qs=oAGoVhmvjhxn7uX6J9%2FOug%3D%3D</t>
   </si>
   <si>
     <t>R3 R18</t>
@@ -397,42 +416,105 @@
     <t>18K</t>
   </si>
   <si>
+    <t>MFR-12FTF52-18K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-18K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-18K?qs=oAGoVhmvjhyrIv61YZaM%252Bw%3D%3D</t>
+  </si>
+  <si>
     <t>R4 R5 R10 R11 R19 R20 R25 R26</t>
   </si>
   <si>
     <t>15K</t>
   </si>
   <si>
+    <t>MFR-12FTF52-15K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-15K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-15K?qs=oAGoVhmvjhxmMJFRswMR%252BA%3D%3D</t>
+  </si>
+  <si>
     <t>R6 R12 R21 R27</t>
   </si>
   <si>
     <t>10K</t>
   </si>
   <si>
+    <t>MFR-12FTF52-10K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-10K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-10K?qs=oAGoVhmvjhzLlUYKKBtdYQ%3D%3D</t>
+  </si>
+  <si>
     <t>R7 R22</t>
   </si>
   <si>
     <t>120K</t>
   </si>
   <si>
+    <t>MFR-12FTF52-120K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-120K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-120K?qs=oAGoVhmvjhymMraGPHdD1w%3D%3D</t>
+  </si>
+  <si>
     <t>R8 R23</t>
   </si>
   <si>
     <t>27K</t>
   </si>
   <si>
+    <t>MFR-12FTF52-27K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-27K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-27K?qs=oAGoVhmvjhyCFqUmM0XEdA%3D%3D</t>
+  </si>
+  <si>
     <t>R9 R24</t>
   </si>
   <si>
     <t>68K</t>
   </si>
   <si>
+    <t>MFR-12FTF52-68K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-68K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-68K?qs=oAGoVhmvjhyL5MsnBkXRfA%3D%3D</t>
+  </si>
+  <si>
     <t>R13 R28</t>
   </si>
   <si>
     <t>200K</t>
   </si>
   <si>
+    <t>MFR-12FTF52-200K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-200K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-200K?qs=oAGoVhmvjhzyXGTT6oqbfw%3D%3D</t>
+  </si>
+  <si>
     <t>R14 R29</t>
   </si>
   <si>
@@ -539,12 +621,21 @@
   </si>
   <si>
     <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/TL072BCP?qs=p6YqzpSxLIxmo8AyZLsP4g%3D%3D</t>
+  </si>
+  <si>
+    <t>Have</t>
+  </si>
+  <si>
+    <t>Bought</t>
+  </si>
+  <si>
+    <t>Need</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1022,8 +1113,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="4"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1069,7 +1161,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1398,940 +1501,1056 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>B2-C2-D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>26</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3">
+        <f t="shared" ref="E3:E25" si="0">B3-C3-D3</f>
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>33</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>34</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>35</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>42</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>43</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>34</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="E5" t="s">
+      <c r="J5" t="s">
         <v>49</v>
       </c>
-      <c r="F5" t="s">
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
         <v>50</v>
       </c>
-      <c r="G5" t="s">
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
         <v>51</v>
       </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="O5" t="s">
         <v>52</v>
       </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
         <v>53</v>
       </c>
-      <c r="L5" t="s">
+      <c r="R5" t="s">
         <v>54</v>
       </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" t="s">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>55</v>
-      </c>
-      <c r="O5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>57</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" t="s">
+      <c r="J6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
+      <c r="K6" t="s">
         <v>60</v>
       </c>
-      <c r="G6" t="s">
+      <c r="L6" t="s">
         <v>61</v>
       </c>
-      <c r="H6" t="s">
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
         <v>62</v>
       </c>
-      <c r="I6" t="s">
+      <c r="O6" t="s">
         <v>63</v>
       </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s">
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>64</v>
-      </c>
-      <c r="L6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>66</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
         <v>68</v>
       </c>
-      <c r="G7" t="s">
+      <c r="L7" t="s">
         <v>69</v>
       </c>
-      <c r="H7" t="s">
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
         <v>70</v>
       </c>
-      <c r="I7" t="s">
+      <c r="O7" t="s">
         <v>71</v>
       </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="P7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" t="s">
         <v>72</v>
       </c>
-      <c r="L7" t="s">
+      <c r="R7" t="s">
         <v>73</v>
       </c>
-      <c r="M7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="S7" t="s">
         <v>74</v>
       </c>
-      <c r="O7" t="s">
+      <c r="T7">
+        <v>4031</v>
+      </c>
+      <c r="U7" t="s">
         <v>75</v>
       </c>
-      <c r="P7" t="s">
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>76</v>
-      </c>
-      <c r="Q7">
-        <v>4031</v>
-      </c>
-      <c r="R7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>78</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" t="s">
         <v>79</v>
       </c>
-      <c r="F8" t="s">
+      <c r="K8" t="s">
         <v>80</v>
       </c>
-      <c r="G8" t="s">
+      <c r="L8">
+        <v>61201021621</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" t="s">
         <v>81</v>
       </c>
-      <c r="H8" t="s">
+      <c r="O8" t="s">
         <v>82</v>
       </c>
-      <c r="I8">
-        <v>61201021621</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="P8" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>83</v>
-      </c>
-      <c r="L8" t="s">
-        <v>84</v>
-      </c>
-      <c r="M8" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>85</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9">
+        <v>598</v>
+      </c>
+      <c r="O9" t="s">
         <v>86</v>
       </c>
-      <c r="F9" t="s">
+      <c r="P9" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" t="s">
         <v>87</v>
       </c>
-      <c r="J9" t="s">
-        <v>76</v>
-      </c>
-      <c r="K9">
-        <v>598</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="R9" t="s">
         <v>88</v>
       </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" t="s">
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>89</v>
-      </c>
-      <c r="O9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>91</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10">
+        <v>1540</v>
+      </c>
+      <c r="O10" t="s">
+        <v>91</v>
+      </c>
+      <c r="P10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10" t="s">
         <v>92</v>
       </c>
-      <c r="F10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J10" t="s">
-        <v>76</v>
-      </c>
-      <c r="K10">
-        <v>1540</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="R10" t="s">
         <v>93</v>
       </c>
-      <c r="M10" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" t="s">
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>94</v>
-      </c>
-      <c r="O10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>96</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" t="s">
         <v>97</v>
       </c>
-      <c r="F11" t="s">
+      <c r="K11" t="s">
         <v>98</v>
       </c>
-      <c r="G11" t="s">
+      <c r="L11" t="s">
         <v>99</v>
       </c>
-      <c r="H11" t="s">
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" t="s">
         <v>100</v>
       </c>
-      <c r="I11" t="s">
+      <c r="O11" t="s">
         <v>101</v>
       </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" t="s">
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>102</v>
-      </c>
-      <c r="L11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>104</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" t="s">
         <v>105</v>
       </c>
-      <c r="F12" t="s">
+      <c r="K12" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
+      <c r="L12" t="s">
         <v>107</v>
       </c>
-      <c r="H12" t="s">
+      <c r="M12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" t="s">
         <v>108</v>
       </c>
-      <c r="I12" t="s">
+      <c r="O12" t="s">
         <v>109</v>
       </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" t="s">
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>110</v>
-      </c>
-      <c r="L12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>112</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" t="s">
         <v>113</v>
       </c>
-      <c r="D13" t="s">
+      <c r="J13" t="s">
         <v>114</v>
       </c>
-      <c r="F13" t="s">
+      <c r="K13" t="s">
         <v>115</v>
       </c>
-      <c r="G13" t="s">
+      <c r="L13" t="s">
         <v>116</v>
       </c>
-      <c r="H13" t="s">
+      <c r="M13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" t="s">
         <v>117</v>
       </c>
-      <c r="I13" t="s">
+      <c r="O13" t="s">
         <v>118</v>
       </c>
-      <c r="J13" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" t="s">
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>119</v>
-      </c>
-      <c r="L13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>121</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" t="s">
         <v>122</v>
       </c>
-      <c r="D14" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" t="s">
-        <v>115</v>
-      </c>
-      <c r="G14" t="s">
-        <v>116</v>
-      </c>
-      <c r="H14" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" t="s">
-        <v>118</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="M14" t="s">
         <v>34</v>
       </c>
-      <c r="K14" t="s">
-        <v>119</v>
-      </c>
-      <c r="L14" t="s">
-        <v>120</v>
+      <c r="N14" t="s">
+        <v>123</v>
+      </c>
+      <c r="O14" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" t="s">
         <v>114</v>
       </c>
-      <c r="F15" t="s">
+      <c r="K15" t="s">
         <v>115</v>
       </c>
-      <c r="G15" t="s">
-        <v>116</v>
-      </c>
-      <c r="H15" t="s">
-        <v>117</v>
-      </c>
-      <c r="I15" t="s">
-        <v>118</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
+        <v>127</v>
+      </c>
+      <c r="M15" t="s">
         <v>34</v>
       </c>
-      <c r="K15" t="s">
-        <v>119</v>
-      </c>
-      <c r="L15" t="s">
-        <v>120</v>
+      <c r="N15" t="s">
+        <v>128</v>
+      </c>
+      <c r="O15" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" t="s">
         <v>114</v>
       </c>
-      <c r="F16" t="s">
+      <c r="K16" t="s">
         <v>115</v>
       </c>
-      <c r="G16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H16" t="s">
-        <v>117</v>
-      </c>
-      <c r="I16" t="s">
-        <v>118</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
+        <v>132</v>
+      </c>
+      <c r="M16" t="s">
         <v>34</v>
       </c>
-      <c r="K16" t="s">
-        <v>119</v>
-      </c>
-      <c r="L16" t="s">
-        <v>120</v>
+      <c r="N16" t="s">
+        <v>133</v>
+      </c>
+      <c r="O16" t="s">
+        <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
-      <c r="C17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" t="s">
         <v>114</v>
       </c>
-      <c r="F17" t="s">
+      <c r="K17" t="s">
         <v>115</v>
       </c>
-      <c r="G17" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" t="s">
-        <v>117</v>
-      </c>
-      <c r="I17" t="s">
-        <v>118</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
+        <v>137</v>
+      </c>
+      <c r="M17" t="s">
         <v>34</v>
       </c>
-      <c r="K17" t="s">
-        <v>119</v>
-      </c>
-      <c r="L17" t="s">
-        <v>120</v>
+      <c r="N17" t="s">
+        <v>138</v>
+      </c>
+      <c r="O17" t="s">
+        <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18" t="s">
         <v>114</v>
       </c>
-      <c r="F18" t="s">
+      <c r="K18" t="s">
         <v>115</v>
       </c>
-      <c r="G18" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I18" t="s">
-        <v>118</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
+        <v>142</v>
+      </c>
+      <c r="M18" t="s">
         <v>34</v>
       </c>
-      <c r="K18" t="s">
-        <v>119</v>
-      </c>
-      <c r="L18" t="s">
-        <v>120</v>
+      <c r="N18" t="s">
+        <v>143</v>
+      </c>
+      <c r="O18" t="s">
+        <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19" t="s">
+        <v>113</v>
+      </c>
+      <c r="J19" t="s">
         <v>114</v>
       </c>
-      <c r="F19" t="s">
+      <c r="K19" t="s">
         <v>115</v>
       </c>
-      <c r="G19" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" t="s">
-        <v>117</v>
-      </c>
-      <c r="I19" t="s">
-        <v>118</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="L19" t="s">
+        <v>147</v>
+      </c>
+      <c r="M19" t="s">
         <v>34</v>
       </c>
-      <c r="K19" t="s">
-        <v>119</v>
-      </c>
-      <c r="L19" t="s">
-        <v>120</v>
+      <c r="N19" t="s">
+        <v>148</v>
+      </c>
+      <c r="O19" t="s">
+        <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
-        <v>134</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>151</v>
+      </c>
+      <c r="G20" t="s">
+        <v>121</v>
+      </c>
+      <c r="I20" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20" t="s">
         <v>114</v>
       </c>
-      <c r="F20" t="s">
+      <c r="K20" t="s">
         <v>115</v>
       </c>
-      <c r="G20" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" t="s">
-        <v>117</v>
-      </c>
-      <c r="I20" t="s">
-        <v>118</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
+        <v>152</v>
+      </c>
+      <c r="M20" t="s">
         <v>34</v>
       </c>
-      <c r="K20" t="s">
-        <v>119</v>
-      </c>
-      <c r="L20" t="s">
-        <v>120</v>
+      <c r="N20" t="s">
+        <v>153</v>
+      </c>
+      <c r="O20" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" t="s">
+        <v>113</v>
+      </c>
+      <c r="J21" t="s">
         <v>114</v>
       </c>
-      <c r="F21" t="s">
+      <c r="K21" t="s">
         <v>115</v>
       </c>
-      <c r="G21" t="s">
-        <v>116</v>
-      </c>
-      <c r="H21" t="s">
-        <v>117</v>
-      </c>
-      <c r="I21" t="s">
-        <v>118</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
+        <v>157</v>
+      </c>
+      <c r="M21" t="s">
         <v>34</v>
       </c>
-      <c r="K21" t="s">
-        <v>119</v>
-      </c>
-      <c r="L21" t="s">
-        <v>120</v>
+      <c r="N21" t="s">
+        <v>158</v>
+      </c>
+      <c r="O21" t="s">
+        <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" t="s">
-        <v>140</v>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="G22" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="H22" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="I22" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="J22" t="s">
+        <v>164</v>
+      </c>
+      <c r="K22" t="s">
+        <v>165</v>
+      </c>
+      <c r="L22" t="s">
+        <v>166</v>
+      </c>
+      <c r="M22" t="s">
         <v>34</v>
       </c>
-      <c r="K22" t="s">
-        <v>144</v>
-      </c>
-      <c r="L22" t="s">
-        <v>145</v>
+      <c r="N22" t="s">
+        <v>167</v>
+      </c>
+      <c r="O22" t="s">
+        <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D23" t="s">
-        <v>147</v>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="G23" t="s">
-        <v>149</v>
-      </c>
-      <c r="H23" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="I23" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="J23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K23" t="s">
+        <v>173</v>
+      </c>
+      <c r="L23" t="s">
+        <v>174</v>
+      </c>
+      <c r="M23" t="s">
         <v>22</v>
       </c>
-      <c r="K23" t="s">
-        <v>152</v>
-      </c>
-      <c r="L23" t="s">
-        <v>153</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
+        <v>175</v>
+      </c>
+      <c r="O23" t="s">
+        <v>176</v>
+      </c>
+      <c r="P23" t="s">
         <v>34</v>
       </c>
-      <c r="N23" t="s">
-        <v>154</v>
-      </c>
-      <c r="O23" t="s">
-        <v>155</v>
-      </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
+        <v>177</v>
+      </c>
+      <c r="R23" t="s">
+        <v>178</v>
+      </c>
+      <c r="S23" t="s">
         <v>24</v>
       </c>
-      <c r="Q23" t="s">
-        <v>156</v>
-      </c>
-      <c r="R23" t="s">
-        <v>157</v>
+      <c r="T23" t="s">
+        <v>179</v>
+      </c>
+      <c r="U23" t="s">
+        <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
-        <v>159</v>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>160</v>
-      </c>
-      <c r="G24" t="s">
-        <v>161</v>
-      </c>
-      <c r="H24" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="I24" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="J24" t="s">
+        <v>184</v>
+      </c>
+      <c r="K24" t="s">
+        <v>185</v>
+      </c>
+      <c r="L24" t="s">
+        <v>186</v>
+      </c>
+      <c r="M24" t="s">
         <v>34</v>
       </c>
-      <c r="K24" t="s">
-        <v>164</v>
-      </c>
-      <c r="L24" t="s">
-        <v>165</v>
+      <c r="N24" t="s">
+        <v>187</v>
+      </c>
+      <c r="O24" t="s">
+        <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
-        <v>167</v>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>168</v>
-      </c>
-      <c r="G25" t="s">
-        <v>169</v>
-      </c>
-      <c r="H25" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="I25" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="J25" t="s">
+        <v>192</v>
+      </c>
+      <c r="K25" t="s">
+        <v>185</v>
+      </c>
+      <c r="L25" t="s">
+        <v>193</v>
+      </c>
+      <c r="M25" t="s">
         <v>34</v>
       </c>
-      <c r="K25" t="s">
-        <v>171</v>
-      </c>
-      <c r="L25" t="s">
-        <v>172</v>
+      <c r="N25" t="s">
+        <v>194</v>
+      </c>
+      <c r="O25" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E25">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Munger re-design - BOM
</commit_message>
<xml_diff>
--- a/modules/Wavefolder/Wavefolder-BOM.xlsx
+++ b/modules/Wavefolder/Wavefolder-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\Wavefolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Wavefolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20497F12-25B4-4B8B-8DD5-B8A35E6B42FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC1F5C7-6C14-4861-B2FA-5141A161464C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="825" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wavefolder-BOM" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="199">
   <si>
     <t>Ref</t>
   </si>
@@ -630,9 +630,6 @@
   </si>
   <si>
     <t>Need</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
 </sst>
 </file>
@@ -1508,16 +1505,16 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="4.1328125" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1624,7 +1621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1663,7 +1660,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1705,7 +1702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1756,7 +1753,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1855,7 +1852,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -1900,7 +1897,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1939,7 +1936,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1978,7 +1975,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -2017,7 +2014,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -2056,7 +2053,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -2098,7 +2095,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -2140,7 +2137,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -2182,7 +2179,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -2192,9 +2189,12 @@
       <c r="C16">
         <v>2</v>
       </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="F16" t="s">
         <v>131</v>
@@ -2224,7 +2224,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -2276,12 +2276,12 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
-        <v>199</v>
-      </c>
-      <c r="E18" t="e">
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>-10</v>
       </c>
       <c r="F18" t="s">
         <v>141</v>
@@ -2311,7 +2311,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>169</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>189</v>
       </c>

</xml_diff>